<commit_message>
update comparison matrices according to latest charactertic evaluation, normalizer is not being set while pmd analysis and hence reports 0 for threshold values
</commit_message>
<xml_diff>
--- a/Comparison_Matrices/compatibility.xlsx
+++ b/Comparison_Matrices/compatibility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guribhangu/development/research/qatch/Comparison_Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0475D8C8-F33E-1A4F-A841-F4BDBFD06776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3830B1D8-AEAB-7349-A5FD-7F31638A160A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{41AF768D-6124-1648-AB05-93B71D6A1BC7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{41AF768D-6124-1648-AB05-93B71D6A1BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J29:J30"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>